<commit_message>
documentation: mapped battery pins to bms
</commit_message>
<xml_diff>
--- a/MEB Battery Pins/MEB-plugs.xlsx
+++ b/MEB Battery Pins/MEB-plugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="35">
   <si>
     <t>Pin Nummer</t>
   </si>
@@ -114,13 +114,28 @@
   </si>
   <si>
     <t>Gesamt+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Kontakte BMS 12s (brauner Stecker)</t>
+  </si>
+  <si>
+    <t>Temp 1</t>
+  </si>
+  <si>
+    <t>Temp 2</t>
+  </si>
+  <si>
+    <t>Beschriftung für 12s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +154,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -268,6 +290,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -344,8 +371,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>118551</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>162094</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
@@ -433,7 +460,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>243841</xdr:colOff>
+      <xdr:colOff>4355</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>174742</xdr:rowOff>
     </xdr:to>
@@ -609,7 +636,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>236221</xdr:colOff>
+      <xdr:colOff>236220</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>52832</xdr:rowOff>
     </xdr:to>
@@ -653,7 +680,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>304599</xdr:colOff>
+      <xdr:colOff>304598</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
@@ -680,6 +707,50 @@
         <a:xfrm>
           <a:off x="10942321" y="1600200"/>
           <a:ext cx="1074218" cy="1348740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>108858</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>76802</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>43544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16328572" y="97972"/>
+          <a:ext cx="1557258" cy="2906486"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -954,19 +1025,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B17:AB35"/>
+  <dimension ref="B17:AE35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="10" width="13.77734375" customWidth="1"/>
-    <col min="11" max="12" width="3.6640625" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" customWidth="1"/>
     <col min="13" max="13" width="1.5546875" customWidth="1"/>
-    <col min="14" max="14" width="3.44140625" customWidth="1"/>
-    <col min="15" max="15" width="4.109375" customWidth="1"/>
+    <col min="14" max="14" width="4.5546875" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" customWidth="1"/>
     <col min="17" max="17" width="15.44140625" customWidth="1"/>
     <col min="18" max="18" width="4.5546875" customWidth="1"/>
     <col min="19" max="19" width="4.33203125" customWidth="1"/>
@@ -979,14 +1051,15 @@
     <col min="26" max="26" width="1.88671875" customWidth="1"/>
     <col min="27" max="27" width="5" customWidth="1"/>
     <col min="28" max="28" width="4.88671875" customWidth="1"/>
+    <col min="29" max="29" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1006,8 +1079,11 @@
       <c r="X18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>12</v>
       </c>
@@ -1026,20 +1102,34 @@
       <c r="I19" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="L19" s="22"/>
-      <c r="N19" s="2"/>
+      <c r="N19" s="24" t="s">
+        <v>3</v>
+      </c>
       <c r="O19" s="3"/>
-      <c r="R19" s="8"/>
+      <c r="R19" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="S19" s="20"/>
-      <c r="U19" s="2"/>
+      <c r="U19" s="24" t="s">
+        <v>29</v>
+      </c>
       <c r="V19" s="3"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="11"/>
       <c r="AA19" s="12"/>
       <c r="AB19" s="13"/>
-    </row>
-    <row r="20" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>13</v>
       </c>
@@ -1058,20 +1148,34 @@
       <c r="I20" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="14"/>
+      <c r="K20" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="L20" s="15"/>
-      <c r="N20" s="2"/>
+      <c r="N20" s="24" t="s">
+        <v>4</v>
+      </c>
       <c r="O20" s="4"/>
-      <c r="R20" s="2"/>
+      <c r="R20" s="24" t="s">
+        <v>4</v>
+      </c>
       <c r="S20" s="4"/>
-      <c r="U20" s="14"/>
+      <c r="U20" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="V20" s="15"/>
       <c r="X20" s="16"/>
       <c r="Y20" s="20"/>
       <c r="AA20" s="5"/>
       <c r="AB20" s="6"/>
-    </row>
-    <row r="21" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD20" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>14</v>
       </c>
@@ -1090,13 +1194,21 @@
       <c r="I21" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="L21" s="20"/>
-      <c r="N21" s="5"/>
+      <c r="N21" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="O21" s="19"/>
-      <c r="R21" s="5"/>
+      <c r="R21" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="S21" s="19"/>
-      <c r="U21" s="17"/>
+      <c r="U21" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="V21" s="20"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="11"/>
@@ -1104,8 +1216,17 @@
         <v>10</v>
       </c>
       <c r="AB21" s="6"/>
-    </row>
-    <row r="22" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>15</v>
       </c>
@@ -1124,20 +1245,34 @@
       <c r="I22" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="L22" s="15"/>
-      <c r="N22" s="8"/>
+      <c r="N22" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="O22" s="4"/>
-      <c r="R22" s="8"/>
+      <c r="R22" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="S22" s="4"/>
-      <c r="U22" s="2"/>
+      <c r="U22" s="24" t="s">
+        <v>16</v>
+      </c>
       <c r="V22" s="15"/>
       <c r="X22" s="18"/>
       <c r="Y22" s="19"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="4"/>
-    </row>
-    <row r="23" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>16</v>
       </c>
@@ -1156,11 +1291,17 @@
       <c r="I23" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="17"/>
+      <c r="K23" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="L23" s="15"/>
-      <c r="N23" s="9"/>
+      <c r="N23" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="O23" s="7"/>
-      <c r="R23" s="9"/>
+      <c r="R23" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="S23" s="7"/>
       <c r="U23" s="14" t="s">
         <v>21</v>
@@ -1170,8 +1311,14 @@
       <c r="Y23" s="11"/>
       <c r="AA23" s="5"/>
       <c r="AB23" s="20"/>
-    </row>
-    <row r="24" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD23" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>17</v>
       </c>
@@ -1190,15 +1337,21 @@
       <c r="I24" t="s">
         <v>8</v>
       </c>
-      <c r="K24" s="17"/>
+      <c r="K24" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="L24" s="11"/>
-      <c r="N24" s="5"/>
+      <c r="N24" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="O24" s="20"/>
       <c r="R24" s="14" t="s">
         <v>21</v>
       </c>
       <c r="S24" s="21"/>
-      <c r="U24" s="17"/>
+      <c r="U24" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="V24" s="15"/>
       <c r="X24" s="17"/>
       <c r="Y24" s="15"/>
@@ -1206,8 +1359,14 @@
         <v>21</v>
       </c>
       <c r="AB24" s="21"/>
-    </row>
-    <row r="25" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD24" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>18</v>
       </c>
@@ -1226,13 +1385,21 @@
       <c r="I25" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="18"/>
+      <c r="K25" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="L25" s="19"/>
-      <c r="N25" s="5"/>
+      <c r="N25" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="O25" s="4"/>
-      <c r="R25" s="5"/>
+      <c r="R25" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="S25" s="20"/>
-      <c r="U25" s="17"/>
+      <c r="U25" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="V25" s="11"/>
       <c r="X25" s="14" t="s">
         <v>21</v>
@@ -1240,8 +1407,14 @@
       <c r="Y25" s="21"/>
       <c r="AA25" s="9"/>
       <c r="AB25" s="7"/>
-    </row>
-    <row r="26" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>19</v>
       </c>
@@ -1260,22 +1433,34 @@
       <c r="I26" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="10"/>
+      <c r="K26" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="L26" s="11"/>
       <c r="N26" s="5" t="s">
         <v>10</v>
       </c>
       <c r="O26" s="6"/>
-      <c r="R26" s="5"/>
+      <c r="R26" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="S26" s="4"/>
-      <c r="U26" s="18"/>
+      <c r="U26" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="V26" s="19"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="15"/>
       <c r="AA26" s="8"/>
       <c r="AB26" s="4"/>
-    </row>
-    <row r="27" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD26" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>20</v>
       </c>
@@ -1306,14 +1491,22 @@
         <v>10</v>
       </c>
       <c r="S27" s="6"/>
-      <c r="U27" s="10"/>
+      <c r="U27" s="27" t="s">
+        <v>28</v>
+      </c>
       <c r="V27" s="11"/>
       <c r="X27" s="17"/>
       <c r="Y27" s="20"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="19"/>
-    </row>
-    <row r="28" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD27" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>21</v>
       </c>
@@ -1332,20 +1525,34 @@
       <c r="I28" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="L28" s="11"/>
-      <c r="N28" s="12"/>
+      <c r="N28" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="O28" s="13"/>
-      <c r="R28" s="5"/>
+      <c r="R28" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="S28" s="6"/>
-      <c r="U28" s="16"/>
+      <c r="U28" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="V28" s="20"/>
       <c r="X28" s="14"/>
       <c r="Y28" s="15"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="4"/>
-    </row>
-    <row r="29" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AD28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>22</v>
       </c>
@@ -1364,20 +1571,39 @@
       <c r="I29" t="s">
         <v>11</v>
       </c>
-      <c r="K29" s="16"/>
+      <c r="K29" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="L29" s="20"/>
-      <c r="N29" s="5"/>
+      <c r="N29" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="O29" s="6"/>
-      <c r="R29" s="12"/>
+      <c r="R29" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="S29" s="13"/>
-      <c r="U29" s="5"/>
+      <c r="U29" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="V29" s="11"/>
       <c r="X29" s="2"/>
       <c r="Y29" s="3"/>
       <c r="AA29" s="8"/>
       <c r="AB29" s="20"/>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="AD29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="R31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>23</v>
       </c>

</xml_diff>